<commit_message>
Adicionada coluna produtos ocupando apenas 1 index por empresa.
</commit_message>
<xml_diff>
--- a/Relatorios/Scraping-ABINEE.xlsx
+++ b/Relatorios/Scraping-ABINEE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\diretorio\Web-Scraping\Relatorios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C9BD70-5E26-4F07-8A37-9184B9943451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABC9FEB-A3BE-4B28-940B-3A295348051E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,8 +54,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,14 +400,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="A14" sqref="A13:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="58.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="58.7109375" style="1"/>
+    <col min="7" max="7" width="58.7109375" style="2"/>
+    <col min="8" max="16384" width="58.7109375" style="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>